<commit_message>
Finished cleaning up tests
</commit_message>
<xml_diff>
--- a/tests/data/tables/generic.genotypes.3.xlsx
+++ b/tests/data/tables/generic.genotypes.3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="trajectory" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t xml:space="preserve">Trajectory</t>
   </si>
@@ -171,9 +171,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>305640</xdr:colOff>
+      <xdr:colOff>304920</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>38520</xdr:rowOff>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -187,7 +187,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="103680" y="1598760"/>
-          <a:ext cx="8076240" cy="6730200"/>
+          <a:ext cx="8075520" cy="6729480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -213,9 +213,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>343800</xdr:colOff>
+      <xdr:colOff>343080</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>60120</xdr:rowOff>
+      <xdr:rowOff>59400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -229,7 +229,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="878400" y="713520"/>
-          <a:ext cx="7994520" cy="6661800"/>
+          <a:ext cx="7993800" cy="6661080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -252,7 +252,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="B4:G4 A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -446,7 +446,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="B4:G4 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -566,8 +566,8 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4:G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -687,7 +687,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="B4:G4 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -744,15 +744,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B4:G4 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="18.9"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -766,12 +770,15 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
     </row>
@@ -786,12 +793,15 @@
         <v>1.83458544342631</v>
       </c>
       <c r="D2" s="0" t="n">
+        <v>1.81558152790223</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>0.830278087225997</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="F2" s="0" t="n">
         <v>1.00815783653297</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="G2" s="0" t="n">
         <v>0.943492689191259</v>
       </c>
     </row>
@@ -806,72 +816,107 @@
         <v>0</v>
       </c>
       <c r="D3" s="0" t="n">
+        <v>0.130761554072711</v>
+      </c>
+      <c r="E3" s="0" t="n">
         <v>1.25554951954802</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="F3" s="0" t="n">
         <v>1.1394684404619</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="G3" s="0" t="n">
         <v>1.19512366294384</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0.830278087225997</v>
+        <v>1.81558152790223</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>1.25554951954802</v>
+        <v>0.130761554072711</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>0.178268246647196</v>
+        <v>1.22163041053492</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>0.103527405716764</v>
+        <v>1.10097133040577</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>1.15938604841685</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1.00815783653297</v>
+        <v>0.830278087225997</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>1.1394684404619</v>
+        <v>1.25554951954802</v>
       </c>
       <c r="D5" s="0" t="n">
+        <v>1.22163041053492</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="0" t="n">
         <v>0.178268246647196</v>
       </c>
-      <c r="E5" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>0.115738277320899</v>
+      <c r="G5" s="0" t="n">
+        <v>0.103527405716764</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1.00815783653297</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1.1394684404619</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1.10097133040577</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.178268246647196</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0.115738277320899</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B7" s="0" t="n">
         <v>0.943492689191259</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C7" s="0" t="n">
         <v>1.19512366294384</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D7" s="0" t="n">
+        <v>1.15938604841685</v>
+      </c>
+      <c r="E7" s="0" t="n">
         <v>0.103527405716764</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="F7" s="0" t="n">
         <v>0.115738277320899</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="G7" s="0" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>